<commit_message>
code to create helpRunTest method
</commit_message>
<xml_diff>
--- a/TestAutomationFramework/src/main/java/ini/TestCases.xlsx
+++ b/TestAutomationFramework/src/main/java/ini/TestCases.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="21030" windowHeight="10650"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +19,34 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Action to do</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Actual result</t>
+  </si>
+  <si>
+    <t>Test result</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM flight WHERE departureAirport='London' AND arrivalAirport='Munich' AND averageTicketPrice&lt;100 AND availableSeats&gt;4</t>
+  </si>
+  <si>
+    <t>1001;2001;3001</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,11 +76,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -331,12 +361,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>